<commit_message>
Add price override to account services
</commit_message>
<xml_diff>
--- a/templates/Account Services.xlsx
+++ b/templates/Account Services.xlsx
@@ -20,14 +20,56 @@
 </workbook>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Price override as a decimal, if you wish to charge a different amount for this service than the base rate.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>The reason for the price override.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Account ID</t>
   </si>
   <si>
     <t>Service ID</t>
   </si>
+  <si>
+    <t>Price Override</t>
+  </si>
+  <si>
+    <t>Price Override Reason</t>
+  </si>
 </sst>
 </file>
 
@@ -41,6 +83,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -67,9 +110,10 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,6 +124,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CCFF"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -117,12 +167,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -203,25 +257,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>27360</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>702720</xdr:colOff>
+      <xdr:colOff>729360</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>86040</xdr:rowOff>
+      <xdr:rowOff>85680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="0" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="360" y="0"/>
-          <a:ext cx="8017560" cy="6263280"/>
+          <a:off x="27360" y="0"/>
+          <a:ext cx="7902720" cy="6262920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -233,11 +287,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0"/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1">
+            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
             <a:t>This template allows you to import services onto accounts.</a:t>
@@ -264,7 +329,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -283,16 +348,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,14 +370,21 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Allow quantity to be set on an account service import
</commit_message>
<xml_diff>
--- a/templates/Account Services.xlsx
+++ b/templates/Account Services.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -35,7 +35,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Price override as a decimal, if you wish to charge a different amount for this service than the base rate.</t>
+          <t xml:space="preserve">Price override as a decimal, if you wish to charge a different amount for this service than the base rate.</t>
         </r>
       </text>
     </comment>
@@ -48,7 +48,21 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>The reason for the price override.</t>
+          <t xml:space="preserve">The reason for the price override.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Defaults to 1 if not provided.
+</t>
         </r>
       </text>
     </comment>
@@ -57,18 +71,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Account ID</t>
+    <t xml:space="preserve">Account ID</t>
   </si>
   <si>
-    <t>Service ID</t>
+    <t xml:space="preserve">Service ID</t>
   </si>
   <si>
-    <t>Price Override</t>
+    <t xml:space="preserve">Price Override</t>
   </si>
   <si>
-    <t>Price Override Reason</t>
+    <t xml:space="preserve">Price Override Reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity</t>
   </si>
 </sst>
 </file>
@@ -76,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -103,7 +120,7 @@
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -263,9 +280,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>729360</xdr:colOff>
+      <xdr:colOff>729000</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>85680</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -275,7 +292,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27360" y="0"/>
-          <a:ext cx="7902720" cy="6262920"/>
+          <a:ext cx="7902360" cy="6262560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -297,7 +314,10 @@
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0"/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:uFill>
                 <a:solidFill>
                   <a:srgbClr val="ffffff"/>
@@ -307,7 +327,17 @@
             </a:rPr>
             <a:t>This template allows you to import services onto accounts.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -323,18 +353,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.34"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -348,19 +378,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -376,11 +406,14 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>